<commit_message>
Excel File 2nd commit
</commit_message>
<xml_diff>
--- a/mansi_raja.xlsx
+++ b/mansi_raja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\work-drive\star\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1593745-98ED-49FE-9BDE-CAC286D92EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14D4FF0-A2CE-4D4E-953E-45A3857FA347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CD598D41-6A10-4912-BDF7-C32B5022E155}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Mansi</t>
   </si>
   <si>
     <t>Raja</t>
+  </si>
+  <si>
+    <t>Drashti</t>
   </si>
 </sst>
 </file>
@@ -382,21 +385,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1645A09-8CD9-4C8F-B034-F83445E60B81}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Excel File 3rd commit
</commit_message>
<xml_diff>
--- a/mansi_raja.xlsx
+++ b/mansi_raja.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\work-drive\star\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14D4FF0-A2CE-4D4E-953E-45A3857FA347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389C265F-AEE5-49AD-8A0D-B90713B1A6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CD598D41-6A10-4912-BDF7-C32B5022E155}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Mansi</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Drashti</t>
+  </si>
+  <si>
+    <t>Pinal</t>
   </si>
 </sst>
 </file>
@@ -385,27 +388,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1645A09-8CD9-4C8F-B034-F83445E60B81}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>